<commit_message>
more ideas + daily log
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787F4A2E-BEB1-483C-B4B1-68CA01466A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA7E584-2B4B-4811-A935-8362F8103E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>DONE Cum</t>
   </si>
@@ -259,12 +259,24 @@
   <si>
     <t>tbd</t>
   </si>
+  <si>
+    <t>meeting</t>
+  </si>
+  <si>
+    <t>Reading 40 SolverCheck: Declarative Testing of Constraints, Reading 41 Grammar-based Whitebox Fuzzing, finding fuzzing with SMT-papers, reading 42 Fuzzing SMT Solvers via Two-Dimensional, Reading 43 Validating SMT Solvers via Semantic Fusion</t>
+  </si>
+  <si>
+    <t>reread FuzzSMT paper 2, reread strom paper 1</t>
+  </si>
+  <si>
+    <t>examen</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,6 +289,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -308,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -320,6 +338,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,70 +554,70 @@
                   <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>155</c:v>
+                  <c:v>170</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>170</c:v>
+                  <c:v>190</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>190</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>228</c:v>
+                  <c:v>248</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>266</c:v>
+                  <c:v>286</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>304</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>342</c:v>
+                  <c:v>362</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>380</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>418</c:v>
+                  <c:v>438</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>456</c:v>
+                  <c:v>476</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>494</c:v>
+                  <c:v>514</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>532</c:v>
+                  <c:v>552</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>570</c:v>
+                  <c:v>590</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>608</c:v>
+                  <c:v>628</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>646</c:v>
+                  <c:v>666</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>684</c:v>
+                  <c:v>704</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>704</c:v>
+                  <c:v>724</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>704</c:v>
+                  <c:v>724</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>704</c:v>
+                  <c:v>724</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>704</c:v>
+                  <c:v>724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -752,70 +771,70 @@
                   <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>115</c:v>
+                  <c:v>122</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -887,6 +906,12 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="5">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="8">
@@ -2020,7 +2045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BD006B-C7A9-475A-9D03-BF9D18D9CC2C}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -2237,7 +2262,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="7">
         <f>Sheet2!C8</f>
         <v>0</v>
       </c>
@@ -2249,6 +2274,9 @@
         <f>SUM($E$3:E9)</f>
         <v>115</v>
       </c>
+      <c r="H9" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -2259,19 +2287,22 @@
         <v>35</v>
       </c>
       <c r="D10">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E10">
         <f>Sheet2!C9</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F10">
         <f>SUM($D$3:D10)</f>
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="G10">
         <f>SUM($E$3:E10)</f>
-        <v>115</v>
+        <v>122</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
@@ -2283,7 +2314,7 @@
         <v>36</v>
       </c>
       <c r="D11">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11">
         <f>Sheet2!C10</f>
@@ -2291,11 +2322,11 @@
       </c>
       <c r="F11">
         <f>SUM($D$3:D11)</f>
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="G11">
         <f>SUM($E$3:E11)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H11" t="s">
         <v>33</v>
@@ -2310,7 +2341,7 @@
         <v>37</v>
       </c>
       <c r="D12">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E12">
         <f>Sheet2!C11</f>
@@ -2318,11 +2349,11 @@
       </c>
       <c r="F12">
         <f>SUM($D$3:D12)</f>
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="G12">
         <f>SUM($E$3:E12)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -2337,7 +2368,7 @@
         <v>38</v>
       </c>
       <c r="D13" s="5">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E13" s="5">
         <f>Sheet2!C12</f>
@@ -2345,11 +2376,11 @@
       </c>
       <c r="F13" s="5">
         <f>SUM($D$3:D13)</f>
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="G13" s="5">
         <f>SUM($E$3:E13)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H13" t="s">
         <v>66</v>
@@ -2372,11 +2403,11 @@
       </c>
       <c r="F14">
         <f>SUM($D$3:D14)</f>
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="G14">
         <f>SUM($E$3:E14)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H14" t="s">
         <v>66</v>
@@ -2399,11 +2430,11 @@
       </c>
       <c r="F15">
         <f>SUM($D$3:D15)</f>
-        <v>228</v>
+        <v>248</v>
       </c>
       <c r="G15">
         <f>SUM($E$3:E15)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H15" t="s">
         <v>66</v>
@@ -2426,11 +2457,11 @@
       </c>
       <c r="F16">
         <f>SUM($D$3:D16)</f>
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="G16">
         <f>SUM($E$3:E16)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H16" t="s">
         <v>66</v>
@@ -2453,11 +2484,11 @@
       </c>
       <c r="F17">
         <f>SUM($D$3:D17)</f>
-        <v>304</v>
+        <v>324</v>
       </c>
       <c r="G17">
         <f>SUM($E$3:E17)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H17" t="s">
         <v>66</v>
@@ -2480,11 +2511,11 @@
       </c>
       <c r="F18">
         <f>SUM($D$3:D18)</f>
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="G18">
         <f>SUM($E$3:E18)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H18" t="s">
         <v>66</v>
@@ -2507,11 +2538,11 @@
       </c>
       <c r="F19">
         <f>SUM($D$3:D19)</f>
-        <v>380</v>
+        <v>400</v>
       </c>
       <c r="G19">
         <f>SUM($E$3:E19)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H19" t="s">
         <v>66</v>
@@ -2534,11 +2565,11 @@
       </c>
       <c r="F20">
         <f>SUM($D$3:D20)</f>
-        <v>418</v>
+        <v>438</v>
       </c>
       <c r="G20">
         <f>SUM($E$3:E20)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H20" t="s">
         <v>66</v>
@@ -2561,11 +2592,11 @@
       </c>
       <c r="F21">
         <f>SUM($D$3:D21)</f>
-        <v>456</v>
+        <v>476</v>
       </c>
       <c r="G21">
         <f>SUM($E$3:E21)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H21" t="s">
         <v>66</v>
@@ -2588,11 +2619,11 @@
       </c>
       <c r="F22">
         <f>SUM($D$3:D22)</f>
-        <v>494</v>
+        <v>514</v>
       </c>
       <c r="G22">
         <f>SUM($E$3:E22)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H22" t="s">
         <v>66</v>
@@ -2615,11 +2646,11 @@
       </c>
       <c r="F23">
         <f>SUM($D$3:D23)</f>
-        <v>532</v>
+        <v>552</v>
       </c>
       <c r="G23">
         <f>SUM($E$3:E23)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H23" t="s">
         <v>66</v>
@@ -2642,11 +2673,11 @@
       </c>
       <c r="F24">
         <f>SUM($D$3:D24)</f>
-        <v>570</v>
+        <v>590</v>
       </c>
       <c r="G24">
         <f>SUM($E$3:E24)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
@@ -2669,11 +2700,11 @@
       </c>
       <c r="F25">
         <f>SUM($D$3:D25)</f>
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="G25">
         <f>SUM($E$3:E25)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H25" t="s">
         <v>34</v>
@@ -2696,11 +2727,11 @@
       </c>
       <c r="F26">
         <f>SUM($D$3:D26)</f>
-        <v>646</v>
+        <v>666</v>
       </c>
       <c r="G26">
         <f>SUM($E$3:E26)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H26" t="s">
         <v>34</v>
@@ -2723,11 +2754,11 @@
       </c>
       <c r="F27">
         <f>SUM($D$3:D27)</f>
-        <v>684</v>
+        <v>704</v>
       </c>
       <c r="G27">
         <f>SUM($E$3:E27)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H27" t="s">
         <v>34</v>
@@ -2750,11 +2781,11 @@
       </c>
       <c r="F28">
         <f>SUM($D$3:D28)</f>
-        <v>704</v>
+        <v>724</v>
       </c>
       <c r="G28">
         <f>SUM($E$3:E28)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H28" t="s">
         <v>34</v>
@@ -2777,11 +2808,11 @@
       </c>
       <c r="F29">
         <f>SUM($D$3:D29)</f>
-        <v>704</v>
+        <v>724</v>
       </c>
       <c r="G29">
         <f>SUM($E$3:E29)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H29" t="s">
         <v>56</v>
@@ -2804,11 +2835,11 @@
       </c>
       <c r="F30">
         <f>SUM($D$3:D30)</f>
-        <v>704</v>
+        <v>724</v>
       </c>
       <c r="G30">
         <f>SUM($E$3:E30)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H30" t="s">
         <v>65</v>
@@ -2831,11 +2862,11 @@
       </c>
       <c r="F31">
         <f>SUM($D$3:D31)</f>
-        <v>704</v>
+        <v>724</v>
       </c>
       <c r="G31">
         <f>SUM($E$3:E31)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H31" t="s">
         <v>65</v>
@@ -2854,11 +2885,11 @@
       </c>
       <c r="D33">
         <f>SUM($D$3:D31)</f>
-        <v>704</v>
+        <v>724</v>
       </c>
       <c r="E33">
         <f>SUM($E$3:E31)</f>
-        <v>115</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2866,8 +2897,8 @@
         <v>43</v>
       </c>
       <c r="B34" s="2">
-        <f>$G$31-F7</f>
-        <v>25</v>
+        <f>$G$31-F10</f>
+        <v>-3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2895,8 +2926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4242F093-96E3-46E1-A347-B0CA60EA4F88}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3144,7 +3175,7 @@
         <v>33</v>
       </c>
       <c r="C7">
-        <f>4+2</f>
+        <f>4+2+0+0+0+0+0</f>
         <v>6</v>
       </c>
       <c r="D7" t="s">
@@ -3153,6 +3184,26 @@
       <c r="E7" t="s">
         <v>62</v>
       </c>
+      <c r="F7" t="str">
+        <f t="shared" ref="E7:J9" si="1">IF($E$33, "Self adaptive Systems", "")</f>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
       <c r="K7" t="s">
         <v>31</v>
       </c>
@@ -3165,6 +3216,38 @@
       <c r="B8">
         <v>34</v>
       </c>
+      <c r="C8">
+        <f>0+0+0+0+0+0+0</f>
+        <v>0</v>
+      </c>
+      <c r="D8" t="str">
+        <f>IF($E$33, "Self adaptive Systems", "")</f>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
       <c r="K8" t="s">
         <v>31</v>
       </c>
@@ -3176,6 +3259,27 @@
       </c>
       <c r="B9">
         <v>35</v>
+      </c>
+      <c r="C9">
+        <f>0+0+7</f>
+        <v>7</v>
+      </c>
+      <c r="D9" t="str">
+        <f>IF($E$33, "Self adaptive Systems", "")</f>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>Self adaptive Systems</v>
+      </c>
+      <c r="F9" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
       </c>
       <c r="K9" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
new sources + daily progress
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFA7E584-2B4B-4811-A935-8362F8103E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7329504A-5A40-4714-9A1C-C876E53455FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
   <si>
     <t>DONE Cum</t>
   </si>
@@ -260,16 +261,22 @@
     <t>tbd</t>
   </si>
   <si>
-    <t>meeting</t>
-  </si>
-  <si>
     <t>Reading 40 SolverCheck: Declarative Testing of Constraints, Reading 41 Grammar-based Whitebox Fuzzing, finding fuzzing with SMT-papers, reading 42 Fuzzing SMT Solvers via Two-Dimensional, Reading 43 Validating SMT Solvers via Semantic Fusion</t>
   </si>
   <si>
-    <t>reread FuzzSMT paper 2, reread strom paper 1</t>
-  </si>
-  <si>
     <t>examen</t>
+  </si>
+  <si>
+    <t>SMT or CP</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t>fuzzing</t>
+  </si>
+  <si>
+    <t>Rereading FuzzSMT Fuzzing and Delta-Debugging SMT Solver, Rereading strom Detecting Critical Bugs in SMT Solvers Using Blackbox Mutational Fuzzing, Reading 44 StringFuzz: A Fuzzer for String Solvers, Rereading 8 KLEE Unassisted and Automatic Generation of High-Coverage, Reading 45 fuzzball Path-Exploration Lifting Hi-Fi Tests for Lo-Fi Emulators, Reading 47 Finding and Understanding Bugs in Software Model Checkers, Reading 48 Differentially Testing Soundness and Precision of Program Analyzers</t>
   </si>
 </sst>
 </file>
@@ -335,10 +342,10 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,70 +778,70 @@
                   <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>122</c:v>
+                  <c:v>128.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2045,7 +2052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BD006B-C7A9-475A-9D03-BF9D18D9CC2C}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
@@ -2057,15 +2064,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2262,7 +2269,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E9" s="6">
         <f>Sheet2!C8</f>
         <v>0</v>
       </c>
@@ -2275,7 +2282,7 @@
         <v>115</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -2291,7 +2298,7 @@
       </c>
       <c r="E10">
         <f>Sheet2!C9</f>
-        <v>7</v>
+        <v>13.5</v>
       </c>
       <c r="F10">
         <f>SUM($D$3:D10)</f>
@@ -2299,7 +2306,7 @@
       </c>
       <c r="G10">
         <f>SUM($E$3:E10)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -2326,7 +2333,7 @@
       </c>
       <c r="G11">
         <f>SUM($E$3:E11)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H11" t="s">
         <v>33</v>
@@ -2353,7 +2360,7 @@
       </c>
       <c r="G12">
         <f>SUM($E$3:E12)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
@@ -2380,7 +2387,7 @@
       </c>
       <c r="G13" s="5">
         <f>SUM($E$3:E13)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H13" t="s">
         <v>66</v>
@@ -2407,7 +2414,7 @@
       </c>
       <c r="G14">
         <f>SUM($E$3:E14)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H14" t="s">
         <v>66</v>
@@ -2434,7 +2441,7 @@
       </c>
       <c r="G15">
         <f>SUM($E$3:E15)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H15" t="s">
         <v>66</v>
@@ -2461,7 +2468,7 @@
       </c>
       <c r="G16">
         <f>SUM($E$3:E16)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H16" t="s">
         <v>66</v>
@@ -2488,7 +2495,7 @@
       </c>
       <c r="G17">
         <f>SUM($E$3:E17)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H17" t="s">
         <v>66</v>
@@ -2515,7 +2522,7 @@
       </c>
       <c r="G18">
         <f>SUM($E$3:E18)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H18" t="s">
         <v>66</v>
@@ -2542,7 +2549,7 @@
       </c>
       <c r="G19">
         <f>SUM($E$3:E19)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H19" t="s">
         <v>66</v>
@@ -2569,7 +2576,7 @@
       </c>
       <c r="G20">
         <f>SUM($E$3:E20)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H20" t="s">
         <v>66</v>
@@ -2596,7 +2603,7 @@
       </c>
       <c r="G21">
         <f>SUM($E$3:E21)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H21" t="s">
         <v>66</v>
@@ -2623,7 +2630,7 @@
       </c>
       <c r="G22">
         <f>SUM($E$3:E22)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H22" t="s">
         <v>66</v>
@@ -2650,7 +2657,7 @@
       </c>
       <c r="G23">
         <f>SUM($E$3:E23)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H23" t="s">
         <v>66</v>
@@ -2677,7 +2684,7 @@
       </c>
       <c r="G24">
         <f>SUM($E$3:E24)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
@@ -2704,7 +2711,7 @@
       </c>
       <c r="G25">
         <f>SUM($E$3:E25)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H25" t="s">
         <v>34</v>
@@ -2731,7 +2738,7 @@
       </c>
       <c r="G26">
         <f>SUM($E$3:E26)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H26" t="s">
         <v>34</v>
@@ -2758,7 +2765,7 @@
       </c>
       <c r="G27">
         <f>SUM($E$3:E27)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H27" t="s">
         <v>34</v>
@@ -2785,7 +2792,7 @@
       </c>
       <c r="G28">
         <f>SUM($E$3:E28)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H28" t="s">
         <v>34</v>
@@ -2812,7 +2819,7 @@
       </c>
       <c r="G29">
         <f>SUM($E$3:E29)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H29" t="s">
         <v>56</v>
@@ -2839,7 +2846,7 @@
       </c>
       <c r="G30">
         <f>SUM($E$3:E30)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H30" t="s">
         <v>65</v>
@@ -2866,7 +2873,7 @@
       </c>
       <c r="G31">
         <f>SUM($E$3:E31)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
       <c r="H31" t="s">
         <v>65</v>
@@ -2889,7 +2896,7 @@
       </c>
       <c r="E33">
         <f>SUM($E$3:E31)</f>
-        <v>122</v>
+        <v>128.5</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2898,7 +2905,7 @@
       </c>
       <c r="B34" s="2">
         <f>$G$31-F10</f>
-        <v>-3</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2926,7 +2933,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4242F093-96E3-46E1-A347-B0CA60EA4F88}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -3261,8 +3268,8 @@
         <v>35</v>
       </c>
       <c r="C9">
-        <f>0+0+7</f>
-        <v>7</v>
+        <f>0+0+7+6.5</f>
+        <v>13.5</v>
       </c>
       <c r="D9" t="str">
         <f>IF($E$33, "Self adaptive Systems", "")</f>
@@ -3273,13 +3280,10 @@
         <v>Self adaptive Systems</v>
       </c>
       <c r="F9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G9" t="s">
-        <v>69</v>
-      </c>
-      <c r="H9" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="K9" t="s">
         <v>31</v>
@@ -3602,4 +3606,213 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{157957EE-64C4-43CE-9071-0561D95D5CE4}">
+  <dimension ref="B2:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <v>16</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>21</v>
+      </c>
+      <c r="D11">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>23</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>24</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>27</v>
+      </c>
+      <c r="D17">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>31</v>
+      </c>
+      <c r="D19">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30">
+        <f>COUNT(C3:C25)</f>
+        <v>23</v>
+      </c>
+      <c r="D30">
+        <f>COUNT(D3:D25)</f>
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:D19">
+    <sortCondition ref="D3:D19"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
daily work, reading 49-50, adding to structure for paper,
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7329504A-5A40-4714-9A1C-C876E53455FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CCFB84-2E38-438F-B7ED-41321E1EEA5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
   <si>
     <t>DONE Cum</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>Rereading FuzzSMT Fuzzing and Delta-Debugging SMT Solver, Rereading strom Detecting Critical Bugs in SMT Solvers Using Blackbox Mutational Fuzzing, Reading 44 StringFuzz: A Fuzzer for String Solvers, Rereading 8 KLEE Unassisted and Automatic Generation of High-Coverage, Reading 45 fuzzball Path-Exploration Lifting Hi-Fi Tests for Lo-Fi Emulators, Reading 47 Finding and Understanding Bugs in Software Model Checkers, Reading 48 Differentially Testing Soundness and Precision of Program Analyzers</t>
+  </si>
+  <si>
+    <t>Reading on minimal unsatisfiable subset, Reading 49 TestMC Testing Model Counters using Differential and Metamorphic Testing, Reading 50 Metamorphic testing of constraint solvers, adding parts to further write on</t>
+  </si>
+  <si>
+    <t>papers about</t>
+  </si>
+  <si>
+    <t>thesis meeting, perperation work</t>
   </si>
 </sst>
 </file>
@@ -333,10 +342,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -561,70 +569,70 @@
                   <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>125</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>150</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>170</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>190</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>210</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>248</c:v>
+                  <c:v>258</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>286</c:v>
+                  <c:v>296</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>324</c:v>
+                  <c:v>334</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>362</c:v>
+                  <c:v>372</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>400</c:v>
+                  <c:v>410</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>438</c:v>
+                  <c:v>448</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>476</c:v>
+                  <c:v>486</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>514</c:v>
+                  <c:v>524</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>552</c:v>
+                  <c:v>562</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>590</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>628</c:v>
+                  <c:v>638</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>666</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>704</c:v>
+                  <c:v>714</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>724</c:v>
+                  <c:v>734</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>724</c:v>
+                  <c:v>734</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>724</c:v>
+                  <c:v>734</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>724</c:v>
+                  <c:v>734</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -778,70 +786,70 @@
                   <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>128.5</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2052,8 +2060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BD006B-C7A9-475A-9D03-BF9D18D9CC2C}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,15 +2072,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2269,7 +2277,7 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <f>Sheet2!C8</f>
         <v>0</v>
       </c>
@@ -2294,19 +2302,19 @@
         <v>35</v>
       </c>
       <c r="D10">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E10">
         <f>Sheet2!C9</f>
-        <v>13.5</v>
+        <v>20</v>
       </c>
       <c r="F10">
         <f>SUM($D$3:D10)</f>
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="G10">
         <f>SUM($E$3:E10)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H10" t="s">
         <v>33</v>
@@ -2321,7 +2329,7 @@
         <v>36</v>
       </c>
       <c r="D11">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E11">
         <f>Sheet2!C10</f>
@@ -2329,11 +2337,11 @@
       </c>
       <c r="F11">
         <f>SUM($D$3:D11)</f>
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="G11">
         <f>SUM($E$3:E11)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H11" t="s">
         <v>33</v>
@@ -2356,38 +2364,38 @@
       </c>
       <c r="F12">
         <f>SUM($D$3:D12)</f>
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="G12">
         <f>SUM($E$3:E12)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="4">
+      <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>44823</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>38</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>20</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f>Sheet2!C12</f>
         <v>0</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f>SUM($D$3:D13)</f>
-        <v>190</v>
-      </c>
-      <c r="G13" s="5">
+        <v>200</v>
+      </c>
+      <c r="G13" s="4">
         <f>SUM($E$3:E13)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H13" t="s">
         <v>66</v>
@@ -2410,11 +2418,11 @@
       </c>
       <c r="F14">
         <f>SUM($D$3:D14)</f>
-        <v>210</v>
+        <v>220</v>
       </c>
       <c r="G14">
         <f>SUM($E$3:E14)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H14" t="s">
         <v>66</v>
@@ -2437,11 +2445,11 @@
       </c>
       <c r="F15">
         <f>SUM($D$3:D15)</f>
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="G15">
         <f>SUM($E$3:E15)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H15" t="s">
         <v>66</v>
@@ -2464,11 +2472,11 @@
       </c>
       <c r="F16">
         <f>SUM($D$3:D16)</f>
-        <v>286</v>
+        <v>296</v>
       </c>
       <c r="G16">
         <f>SUM($E$3:E16)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H16" t="s">
         <v>66</v>
@@ -2491,11 +2499,11 @@
       </c>
       <c r="F17">
         <f>SUM($D$3:D17)</f>
-        <v>324</v>
+        <v>334</v>
       </c>
       <c r="G17">
         <f>SUM($E$3:E17)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H17" t="s">
         <v>66</v>
@@ -2518,11 +2526,11 @@
       </c>
       <c r="F18">
         <f>SUM($D$3:D18)</f>
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="G18">
         <f>SUM($E$3:E18)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H18" t="s">
         <v>66</v>
@@ -2545,11 +2553,11 @@
       </c>
       <c r="F19">
         <f>SUM($D$3:D19)</f>
-        <v>400</v>
+        <v>410</v>
       </c>
       <c r="G19">
         <f>SUM($E$3:E19)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H19" t="s">
         <v>66</v>
@@ -2572,11 +2580,11 @@
       </c>
       <c r="F20">
         <f>SUM($D$3:D20)</f>
-        <v>438</v>
+        <v>448</v>
       </c>
       <c r="G20">
         <f>SUM($E$3:E20)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H20" t="s">
         <v>66</v>
@@ -2599,11 +2607,11 @@
       </c>
       <c r="F21">
         <f>SUM($D$3:D21)</f>
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="G21">
         <f>SUM($E$3:E21)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H21" t="s">
         <v>66</v>
@@ -2626,11 +2634,11 @@
       </c>
       <c r="F22">
         <f>SUM($D$3:D22)</f>
-        <v>514</v>
+        <v>524</v>
       </c>
       <c r="G22">
         <f>SUM($E$3:E22)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H22" t="s">
         <v>66</v>
@@ -2653,11 +2661,11 @@
       </c>
       <c r="F23">
         <f>SUM($D$3:D23)</f>
-        <v>552</v>
+        <v>562</v>
       </c>
       <c r="G23">
         <f>SUM($E$3:E23)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H23" t="s">
         <v>66</v>
@@ -2680,11 +2688,11 @@
       </c>
       <c r="F24">
         <f>SUM($D$3:D24)</f>
-        <v>590</v>
+        <v>600</v>
       </c>
       <c r="G24">
         <f>SUM($E$3:E24)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H24" t="s">
         <v>35</v>
@@ -2707,11 +2715,11 @@
       </c>
       <c r="F25">
         <f>SUM($D$3:D25)</f>
-        <v>628</v>
+        <v>638</v>
       </c>
       <c r="G25">
         <f>SUM($E$3:E25)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H25" t="s">
         <v>34</v>
@@ -2734,11 +2742,11 @@
       </c>
       <c r="F26">
         <f>SUM($D$3:D26)</f>
-        <v>666</v>
+        <v>676</v>
       </c>
       <c r="G26">
         <f>SUM($E$3:E26)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H26" t="s">
         <v>34</v>
@@ -2761,11 +2769,11 @@
       </c>
       <c r="F27">
         <f>SUM($D$3:D27)</f>
-        <v>704</v>
+        <v>714</v>
       </c>
       <c r="G27">
         <f>SUM($E$3:E27)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H27" t="s">
         <v>34</v>
@@ -2788,11 +2796,11 @@
       </c>
       <c r="F28">
         <f>SUM($D$3:D28)</f>
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="G28">
         <f>SUM($E$3:E28)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H28" t="s">
         <v>34</v>
@@ -2815,11 +2823,11 @@
       </c>
       <c r="F29">
         <f>SUM($D$3:D29)</f>
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="G29">
         <f>SUM($E$3:E29)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H29" t="s">
         <v>56</v>
@@ -2842,11 +2850,11 @@
       </c>
       <c r="F30">
         <f>SUM($D$3:D30)</f>
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="G30">
         <f>SUM($E$3:E30)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H30" t="s">
         <v>65</v>
@@ -2869,11 +2877,11 @@
       </c>
       <c r="F31">
         <f>SUM($D$3:D31)</f>
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="G31">
         <f>SUM($E$3:E31)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
       <c r="H31" t="s">
         <v>65</v>
@@ -2886,26 +2894,22 @@
       <c r="A33" t="s">
         <v>27</v>
       </c>
-      <c r="B33" s="2">
-        <f>COUNT(B3:B31)</f>
-        <v>29</v>
-      </c>
       <c r="D33">
         <f>SUM($D$3:D31)</f>
-        <v>724</v>
+        <v>734</v>
       </c>
       <c r="E33">
         <f>SUM($E$3:E31)</f>
-        <v>128.5</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34">
         <f>$G$31-F10</f>
-        <v>3.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2933,8 +2937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4242F093-96E3-46E1-A347-B0CA60EA4F88}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2948,7 +2952,7 @@
     <col min="7" max="7" width="23.42578125" customWidth="1"/>
     <col min="8" max="8" width="26.28515625" customWidth="1"/>
     <col min="9" max="9" width="32.7109375" customWidth="1"/>
-    <col min="10" max="10" width="46" customWidth="1"/>
+    <col min="10" max="10" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -3073,7 +3077,7 @@
         <f>4+2+4+4+4+4+4</f>
         <v>26</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>39</v>
       </c>
       <c r="E4" t="s">
@@ -3268,8 +3272,8 @@
         <v>35</v>
       </c>
       <c r="C9">
-        <f>0+0+7+6.5</f>
-        <v>13.5</v>
+        <f>0+0+7+7+2+4</f>
+        <v>20</v>
       </c>
       <c r="D9" t="str">
         <f>IF($E$33, "Self adaptive Systems", "")</f>
@@ -3285,6 +3289,12 @@
       <c r="G9" t="s">
         <v>72</v>
       </c>
+      <c r="H9" t="s">
+        <v>75</v>
+      </c>
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
       <c r="K9" t="s">
         <v>31</v>
       </c>
@@ -3585,16 +3595,12 @@
       <c r="A32" s="1"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
       <c r="D33" t="s">
         <v>30</v>
       </c>
       <c r="E33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
@@ -3613,16 +3619,20 @@
   <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>74</v>
+      </c>
       <c r="C2" t="s">
         <v>71</v>
       </c>
@@ -3630,7 +3640,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3">
         <v>3</v>
       </c>
@@ -3638,7 +3648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4">
         <v>4</v>
       </c>
@@ -3646,7 +3656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>7</v>
       </c>
@@ -3654,7 +3664,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>8</v>
       </c>
@@ -3662,7 +3672,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>10</v>
       </c>
@@ -3670,7 +3680,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>12</v>
       </c>
@@ -3678,7 +3688,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>14</v>
       </c>
@@ -3686,7 +3696,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C10">
         <v>16</v>
       </c>
@@ -3694,7 +3704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>21</v>
       </c>
@@ -3702,7 +3712,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C12">
         <v>22</v>
       </c>
@@ -3710,7 +3720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C13">
         <v>23</v>
       </c>
@@ -3718,7 +3728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C14">
         <v>24</v>
       </c>
@@ -3726,7 +3736,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C15">
         <v>25</v>
       </c>
@@ -3734,7 +3744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C16">
         <v>26</v>
       </c>
@@ -3770,11 +3780,17 @@
       <c r="C20">
         <v>32</v>
       </c>
+      <c r="D20">
+        <v>49</v>
+      </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>34</v>
       </c>
+      <c r="D21">
+        <v>50</v>
+      </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22">
@@ -3796,17 +3812,27 @@
         <v>46</v>
       </c>
     </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>50</v>
+      </c>
+    </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>70</v>
       </c>
       <c r="C30">
-        <f>COUNT(C3:C25)</f>
-        <v>23</v>
+        <f>COUNT(C3:C27)</f>
+        <v>25</v>
       </c>
       <c r="D30">
         <f>COUNT(D3:D25)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
proofreading and smaller changes to chapter around CP
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5F1EBF-74EA-438A-A74E-DC6E9AC79E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FE83E5-F1EF-4E43-9719-2A0EFEC2DC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="270" windowWidth="25440" windowHeight="15390" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="28680" yWindow="240" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="83">
   <si>
     <t>DONE Cum</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Writing about SAT, SMT, Reading 71 CVC3, Reading 72 A System for Solving Constraint Satisfaction Problems with SMT bofill-sat10.pdf</t>
+  </si>
+  <si>
+    <t>Writing conclusion of chapter CP, proofreading chapter CP, partial reading 73 Simplify A Theorem Prover for Program Checking 1066100.1066102.pdf</t>
   </si>
 </sst>
 </file>
@@ -596,61 +599,61 @@
                   <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>205</c:v>
+                  <c:v>215</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>225</c:v>
+                  <c:v>255</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>263</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>283</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>321</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>359</c:v>
+                  <c:v>375</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>397</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>435</c:v>
+                  <c:v>455</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>473</c:v>
+                  <c:v>495</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>511</c:v>
+                  <c:v>535</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>549</c:v>
+                  <c:v>575</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>587</c:v>
+                  <c:v>615</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>625</c:v>
+                  <c:v>655</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>663</c:v>
+                  <c:v>695</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>701</c:v>
+                  <c:v>735</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>721</c:v>
+                  <c:v>775</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>721</c:v>
+                  <c:v>815</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>721</c:v>
+                  <c:v>815</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>721</c:v>
+                  <c:v>815</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -813,61 +816,61 @@
                   <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>200</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1742,14 +1745,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
+      <xdr:colOff>333375</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
@@ -2078,8 +2081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BD006B-C7A9-475A-9D03-BF9D18D9CC2C}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2401,22 +2404,22 @@
         <v>38</v>
       </c>
       <c r="D13" s="4">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E13" s="4">
         <f>Sheet2!C12</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F13" s="4">
         <f>SUM($D$3:D13)</f>
-        <v>205</v>
+        <v>215</v>
       </c>
       <c r="G13" s="4">
         <f>SUM($E$3:E13)</f>
-        <v>200</v>
-      </c>
-      <c r="H13" t="s">
-        <v>61</v>
+        <v>207</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -2428,7 +2431,7 @@
         <v>39</v>
       </c>
       <c r="D14">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <f>Sheet2!C13</f>
@@ -2436,11 +2439,11 @@
       </c>
       <c r="F14">
         <f>SUM($D$3:D14)</f>
-        <v>225</v>
+        <v>255</v>
       </c>
       <c r="G14">
         <f>SUM($E$3:E14)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H14" t="s">
         <v>61</v>
@@ -2455,7 +2458,7 @@
         <v>40</v>
       </c>
       <c r="D15">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E15">
         <f>Sheet2!C14</f>
@@ -2463,11 +2466,11 @@
       </c>
       <c r="F15">
         <f>SUM($D$3:D15)</f>
-        <v>263</v>
+        <v>295</v>
       </c>
       <c r="G15">
         <f>SUM($E$3:E15)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H15" t="s">
         <v>61</v>
@@ -2490,11 +2493,11 @@
       </c>
       <c r="F16">
         <f>SUM($D$3:D16)</f>
-        <v>283</v>
+        <v>315</v>
       </c>
       <c r="G16">
         <f>SUM($E$3:E16)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H16" t="s">
         <v>61</v>
@@ -2509,7 +2512,7 @@
         <v>42</v>
       </c>
       <c r="D17">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="E17">
         <f>Sheet2!C16</f>
@@ -2517,11 +2520,11 @@
       </c>
       <c r="F17">
         <f>SUM($D$3:D17)</f>
-        <v>321</v>
+        <v>335</v>
       </c>
       <c r="G17">
         <f>SUM($E$3:E17)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H17" t="s">
         <v>61</v>
@@ -2536,7 +2539,7 @@
         <v>43</v>
       </c>
       <c r="D18">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <f>Sheet2!C17</f>
@@ -2544,11 +2547,11 @@
       </c>
       <c r="F18">
         <f>SUM($D$3:D18)</f>
-        <v>359</v>
+        <v>375</v>
       </c>
       <c r="G18">
         <f>SUM($E$3:E18)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H18" t="s">
         <v>61</v>
@@ -2563,7 +2566,7 @@
         <v>44</v>
       </c>
       <c r="D19">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E19">
         <f>Sheet2!C18</f>
@@ -2571,11 +2574,11 @@
       </c>
       <c r="F19">
         <f>SUM($D$3:D19)</f>
-        <v>397</v>
+        <v>415</v>
       </c>
       <c r="G19">
         <f>SUM($E$3:E19)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H19" t="s">
         <v>61</v>
@@ -2590,7 +2593,7 @@
         <v>45</v>
       </c>
       <c r="D20">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E20">
         <f>Sheet2!C19</f>
@@ -2598,11 +2601,11 @@
       </c>
       <c r="F20">
         <f>SUM($D$3:D20)</f>
-        <v>435</v>
+        <v>455</v>
       </c>
       <c r="G20">
         <f>SUM($E$3:E20)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H20" t="s">
         <v>61</v>
@@ -2617,7 +2620,7 @@
         <v>46</v>
       </c>
       <c r="D21">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E21">
         <f>Sheet2!C20</f>
@@ -2625,11 +2628,11 @@
       </c>
       <c r="F21">
         <f>SUM($D$3:D21)</f>
-        <v>473</v>
+        <v>495</v>
       </c>
       <c r="G21">
         <f>SUM($E$3:E21)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H21" t="s">
         <v>61</v>
@@ -2644,7 +2647,7 @@
         <v>47</v>
       </c>
       <c r="D22">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E22">
         <f>Sheet2!C21</f>
@@ -2652,11 +2655,11 @@
       </c>
       <c r="F22">
         <f>SUM($D$3:D22)</f>
-        <v>511</v>
+        <v>535</v>
       </c>
       <c r="G22">
         <f>SUM($E$3:E22)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H22" t="s">
         <v>61</v>
@@ -2671,7 +2674,7 @@
         <v>48</v>
       </c>
       <c r="D23">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <f>Sheet2!C22</f>
@@ -2679,11 +2682,11 @@
       </c>
       <c r="F23">
         <f>SUM($D$3:D23)</f>
-        <v>549</v>
+        <v>575</v>
       </c>
       <c r="G23">
         <f>SUM($E$3:E23)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H23" t="s">
         <v>61</v>
@@ -2698,7 +2701,7 @@
         <v>49</v>
       </c>
       <c r="D24">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <f>Sheet2!C23</f>
@@ -2706,11 +2709,11 @@
       </c>
       <c r="F24">
         <f>SUM($D$3:D24)</f>
-        <v>587</v>
+        <v>615</v>
       </c>
       <c r="G24">
         <f>SUM($E$3:E24)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H24" t="s">
         <v>30</v>
@@ -2725,7 +2728,7 @@
         <v>50</v>
       </c>
       <c r="D25">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E25">
         <f>Sheet2!C24</f>
@@ -2733,11 +2736,11 @@
       </c>
       <c r="F25">
         <f>SUM($D$3:D25)</f>
-        <v>625</v>
+        <v>655</v>
       </c>
       <c r="G25">
         <f>SUM($E$3:E25)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
@@ -2752,7 +2755,7 @@
         <v>51</v>
       </c>
       <c r="D26">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E26">
         <f>Sheet2!C25</f>
@@ -2760,11 +2763,11 @@
       </c>
       <c r="F26">
         <f>SUM($D$3:D26)</f>
-        <v>663</v>
+        <v>695</v>
       </c>
       <c r="G26">
         <f>SUM($E$3:E26)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H26" t="s">
         <v>29</v>
@@ -2779,7 +2782,7 @@
         <v>52</v>
       </c>
       <c r="D27">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E27">
         <f>Sheet2!C26</f>
@@ -2787,11 +2790,11 @@
       </c>
       <c r="F27">
         <f>SUM($D$3:D27)</f>
-        <v>701</v>
+        <v>735</v>
       </c>
       <c r="G27">
         <f>SUM($E$3:E27)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H27" t="s">
         <v>29</v>
@@ -2806,7 +2809,7 @@
         <v>1</v>
       </c>
       <c r="D28">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E28">
         <f>Sheet2!C27</f>
@@ -2814,11 +2817,11 @@
       </c>
       <c r="F28">
         <f>SUM($D$3:D28)</f>
-        <v>721</v>
+        <v>775</v>
       </c>
       <c r="G28">
         <f>SUM($E$3:E28)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H28" t="s">
         <v>29</v>
@@ -2833,7 +2836,7 @@
         <v>2</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="E29">
         <f>Sheet2!C28</f>
@@ -2841,11 +2844,11 @@
       </c>
       <c r="F29">
         <f>SUM($D$3:D29)</f>
-        <v>721</v>
+        <v>815</v>
       </c>
       <c r="G29">
         <f>SUM($E$3:E29)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H29" t="s">
         <v>51</v>
@@ -2868,11 +2871,11 @@
       </c>
       <c r="F30">
         <f>SUM($D$3:D30)</f>
-        <v>721</v>
+        <v>815</v>
       </c>
       <c r="G30">
         <f>SUM($E$3:E30)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H30" t="s">
         <v>60</v>
@@ -2895,11 +2898,11 @@
       </c>
       <c r="F31">
         <f>SUM($D$3:D31)</f>
-        <v>721</v>
+        <v>815</v>
       </c>
       <c r="G31">
         <f>SUM($E$3:E31)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="H31" t="s">
         <v>60</v>
@@ -2914,11 +2917,11 @@
       </c>
       <c r="D33">
         <f>SUM($D$3:D31)</f>
-        <v>721</v>
+        <v>815</v>
       </c>
       <c r="E33">
         <f>SUM($E$3:E31)</f>
-        <v>200</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2926,8 +2929,8 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <f>$G$31-F12</f>
-        <v>15</v>
+        <f>$G$31-F13</f>
+        <v>-8</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2955,8 +2958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4242F093-96E3-46E1-A347-B0CA60EA4F88}">
   <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,7 +3370,7 @@
         <v>37</v>
       </c>
       <c r="C11">
-        <f>8+7+5+6</f>
+        <f>8+7+5+6+0+0+0</f>
         <v>26</v>
       </c>
       <c r="D11" t="s">
@@ -3406,13 +3409,16 @@
       <c r="B12">
         <v>38</v>
       </c>
+      <c r="C12">
+        <f>0+7</f>
+        <v>7</v>
+      </c>
       <c r="D12" t="str">
         <f>IF(E33, "kot verhuis", "")</f>
         <v>kot verhuis</v>
       </c>
-      <c r="G12" t="str">
-        <f>IF(E33, "onderwijsnamiddag", "")</f>
-        <v>onderwijsnamiddag</v>
+      <c r="E12" t="s">
+        <v>82</v>
       </c>
       <c r="K12" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Bonus late night session
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33381379-3EFB-4E8E-9217-26837BD82E8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD30636C-7878-49C7-8383-F8C99DCAAC01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="28680" yWindow="240" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
     <t>Mostly making presentation for M2 (rough day)</t>
   </si>
   <si>
-    <t xml:space="preserve">building differential testing </t>
+    <t>building differential testing, debugging some errors (thanks to Linux for OOM killer)</t>
   </si>
 </sst>
 </file>
@@ -977,40 +977,40 @@
                   <c:v>367</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>389</c:v>
+                  <c:v>391</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2778,7 +2778,7 @@
       </c>
       <c r="E18">
         <f>Sheet2!C17</f>
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F18">
         <f>SUM($D$3:D18)</f>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="G18">
         <f>SUM($E$3:E18)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H18" t="s">
         <v>94</v>
@@ -2813,7 +2813,7 @@
       </c>
       <c r="G19">
         <f>SUM($E$3:E19)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H19" t="s">
         <v>95</v>
@@ -2840,7 +2840,7 @@
       </c>
       <c r="G20">
         <f>SUM($E$3:E20)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H20" t="s">
         <v>96</v>
@@ -2867,7 +2867,7 @@
       </c>
       <c r="G21">
         <f>SUM($E$3:E21)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H21" t="s">
         <v>110</v>
@@ -2894,7 +2894,7 @@
       </c>
       <c r="G22">
         <f>SUM($E$3:E22)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H22" t="s">
         <v>110</v>
@@ -2921,7 +2921,7 @@
       </c>
       <c r="G23">
         <f>SUM($E$3:E23)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H23" t="s">
         <v>30</v>
@@ -2948,7 +2948,7 @@
       </c>
       <c r="G24">
         <f>SUM($E$3:E24)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H24" t="s">
         <v>29</v>
@@ -2975,7 +2975,7 @@
       </c>
       <c r="G25">
         <f>SUM($E$3:E25)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
@@ -3002,7 +3002,7 @@
       </c>
       <c r="G26">
         <f>SUM($E$3:E26)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H26" t="s">
         <v>98</v>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="G27">
         <f>SUM($E$3:E27)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H27" t="s">
         <v>29</v>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="G28">
         <f>SUM($E$3:E28)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H28" t="s">
         <v>114</v>
@@ -3083,7 +3083,7 @@
       </c>
       <c r="G29">
         <f>SUM($E$3:E29)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="H29" t="s">
         <v>89</v>
@@ -3111,7 +3111,7 @@
       </c>
       <c r="E31">
         <f>SUM($E$3:E30)</f>
-        <v>389</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3120,7 +3120,7 @@
       </c>
       <c r="B32">
         <f>E31-F18</f>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -3149,7 +3149,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18:G23"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3782,8 +3782,8 @@
         <v>43</v>
       </c>
       <c r="C17">
-        <f>9+5+8</f>
-        <v>22</v>
+        <f>9+5+10</f>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
adding 4 listings tot the text
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C149F07C-EBEC-46F4-B4B4-48DD2651DCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFFAA59F-B851-41EC-A6FC-D03FCBCF17AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="240" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -515,7 +515,7 @@
     <t>weird DEADLINE academisch secretaris</t>
   </si>
   <si>
-    <t>replacing badly cropt image on front page, rereading guidelines_thesis.pdf, moving caption of tables</t>
+    <t>replacing badly cropt image on front page, rereading guidelines_thesis.pdf, moving caption of tables, add listings to some bug explanations</t>
   </si>
 </sst>
 </file>
@@ -1100,25 +1100,25 @@
                   <c:v>557</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>606</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>606</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>606</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>606</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>606</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>606</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>606</c:v>
+                  <c:v>610</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2425,7 +2425,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3021,7 +3021,7 @@
       </c>
       <c r="E23">
         <f>Sheet2!C22</f>
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F23">
         <f>SUM($D$3:D23)</f>
@@ -3029,7 +3029,7 @@
       </c>
       <c r="G23">
         <f>SUM($E$3:E23)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H23" t="s">
         <v>150</v>
@@ -3056,7 +3056,7 @@
       </c>
       <c r="G24">
         <f>SUM($E$3:E24)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H24" t="s">
         <v>29</v>
@@ -3083,7 +3083,7 @@
       </c>
       <c r="G25">
         <f>SUM($E$3:E25)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H25" t="s">
         <v>29</v>
@@ -3110,7 +3110,7 @@
       </c>
       <c r="G26">
         <f>SUM($E$3:E26)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H26" t="s">
         <v>94</v>
@@ -3137,7 +3137,7 @@
       </c>
       <c r="G27">
         <f>SUM($E$3:E27)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H27" t="s">
         <v>29</v>
@@ -3164,7 +3164,7 @@
       </c>
       <c r="G28">
         <f>SUM($E$3:E28)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H28" t="s">
         <v>109</v>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="G29">
         <f>SUM($E$3:E29)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
       <c r="H29" t="s">
         <v>88</v>
@@ -3222,7 +3222,7 @@
       </c>
       <c r="E31">
         <f>SUM($E$3:E30)</f>
-        <v>606</v>
+        <v>610</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3230,8 +3230,8 @@
         <v>37</v>
       </c>
       <c r="B32">
-        <f>E31-F23</f>
-        <v>64</v>
+        <f>E31-F24</f>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
@@ -3264,7 +3264,7 @@
   <dimension ref="A1:K35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4080,8 +4080,8 @@
         <v>48</v>
       </c>
       <c r="C22">
-        <f>9+9+9+9+9+4</f>
-        <v>49</v>
+        <f>9+9+9+9+9+4+4</f>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
new feedback = better txt
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A716325C-88F8-4709-8E8B-DB05EDE74266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD318933-3EAA-4083-AB69-DB8DC5DE93C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="28680" yWindow="240" windowWidth="25440" windowHeight="15390" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="160">
   <si>
     <t>DONE Cum</t>
   </si>
@@ -534,6 +534,9 @@
   </si>
   <si>
     <t>rereading assignments, updating found bugs</t>
+  </si>
+  <si>
+    <t>processing amazing feedback from Ignace Bleukx</t>
   </si>
 </sst>
 </file>
@@ -1121,22 +1124,22 @@
                   <c:v>610</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>641</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>641</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>641</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>641</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>641</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>641</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3066,7 +3069,7 @@
       </c>
       <c r="E24">
         <f>Sheet2!C23</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F24">
         <f>SUM($D$3:D24)</f>
@@ -3074,7 +3077,7 @@
       </c>
       <c r="G24">
         <f>SUM($E$3:E24)</f>
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="H24" t="s">
         <v>155</v>
@@ -3101,7 +3104,7 @@
       </c>
       <c r="G25">
         <f>SUM($E$3:E25)</f>
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="H25" t="s">
         <v>108</v>
@@ -3128,7 +3131,7 @@
       </c>
       <c r="G26">
         <f>SUM($E$3:E26)</f>
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="H26" t="s">
         <v>156</v>
@@ -3155,7 +3158,7 @@
       </c>
       <c r="G27">
         <f>SUM($E$3:E27)</f>
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="H27" t="s">
         <v>29</v>
@@ -3182,7 +3185,7 @@
       </c>
       <c r="G28">
         <f>SUM($E$3:E28)</f>
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="H28" t="s">
         <v>108</v>
@@ -3209,7 +3212,7 @@
       </c>
       <c r="G29">
         <f>SUM($E$3:E29)</f>
-        <v>641</v>
+        <v>645</v>
       </c>
       <c r="H29" t="s">
         <v>88</v>
@@ -3240,7 +3243,7 @@
       </c>
       <c r="E31">
         <f>SUM($E$3:E30)</f>
-        <v>641</v>
+        <v>645</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3249,7 +3252,7 @@
       </c>
       <c r="B32">
         <f>E31-F24</f>
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -3279,7 +3282,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4132,8 +4135,8 @@
         <v>49</v>
       </c>
       <c r="C23">
-        <f>9+8+4+7+3</f>
-        <v>31</v>
+        <f>9+8+4+7+3+0+4</f>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
         <v>152</v>
@@ -4149,6 +4152,9 @@
       </c>
       <c r="H23" t="s">
         <v>158</v>
+      </c>
+      <c r="J23" t="s">
+        <v>159</v>
       </c>
       <c r="K23" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
camelCase Titles and cleaning up document outline
Filled in the English template as well (not planning to use it), adding camelCase to titles, splitting up list of images and tables, consistent plural in similar tables
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruben\Desktop\Thesis\Masterproef-paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D86601-7046-466A-9E46-C8FFD145A125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AFEF85-CB9A-4513-BF7B-14577FB9B5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A8770C7F-A2D2-4D88-ABBC-8B425DE253D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="173">
   <si>
     <t>DONE Cum</t>
   </si>
@@ -482,9 +482,6 @@
     <t>academisch secretaris luc.vaneycken@kuleuven.be</t>
   </si>
   <si>
-    <t>Poster</t>
-  </si>
-  <si>
     <t>finishing writing implmentation, writing about the results (running the fuzzer tests, preventing frequent reoccuring bugs, describing double not bug), helping with bug 165</t>
   </si>
   <si>
@@ -521,9 +518,6 @@
     <t>finishing the thext</t>
   </si>
   <si>
-    <t>Proofreading + asking permission</t>
-  </si>
-  <si>
     <t>Processing first feedbacks, creating possible titles, reading how the poster should be made, adding rough outline of poster, fixing last todo's</t>
   </si>
   <si>
@@ -579,6 +573,9 @@
   </si>
   <si>
     <t>processing new feedback</t>
+  </si>
+  <si>
+    <t>Proofreading, poster</t>
   </si>
 </sst>
 </file>
@@ -1310,9 +1307,6 @@
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="23">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="25">
@@ -2487,7 +2481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56BD006B-C7A9-475A-9D03-BF9D18D9CC2C}">
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
@@ -3095,7 +3089,7 @@
         <v>610</v>
       </c>
       <c r="H23" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3122,7 +3116,7 @@
         <v>645</v>
       </c>
       <c r="H24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3176,7 +3170,7 @@
         <v>701</v>
       </c>
       <c r="H26" t="s">
-        <v>154</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3202,9 +3196,6 @@
         <f>SUM($E$3:E27)</f>
         <v>703</v>
       </c>
-      <c r="H27" t="s">
-        <v>29</v>
-      </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
@@ -3230,7 +3221,7 @@
         <v>707</v>
       </c>
       <c r="H28" t="s">
-        <v>107</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3271,9 +3262,6 @@
       <c r="D30">
         <v>0</v>
       </c>
-      <c r="H30" t="s">
-        <v>141</v>
-      </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -3293,8 +3281,8 @@
         <v>37</v>
       </c>
       <c r="B32">
-        <f>E31-F25</f>
-        <v>95</v>
+        <f>E31-F28</f>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -3322,7 +3310,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4242F093-96E3-46E1-A347-B0CA60EA4F88}">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F27" sqref="F27"/>
     </sheetView>
@@ -4144,25 +4132,25 @@
         <v>53</v>
       </c>
       <c r="D22" t="s">
+        <v>141</v>
+      </c>
+      <c r="E22" t="s">
         <v>142</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>143</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>144</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>145</v>
       </c>
-      <c r="H22" t="s">
+      <c r="I22" t="s">
         <v>146</v>
       </c>
-      <c r="I22" t="s">
-        <v>147</v>
-      </c>
       <c r="J22" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K22" t="s">
         <v>26</v>
@@ -4181,22 +4169,22 @@
         <v>35</v>
       </c>
       <c r="D23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" t="s">
         <v>150</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>151</v>
       </c>
-      <c r="F23" t="s">
-        <v>152</v>
-      </c>
       <c r="G23" t="s">
+        <v>153</v>
+      </c>
+      <c r="H23" t="s">
+        <v>154</v>
+      </c>
+      <c r="J23" t="s">
         <v>155</v>
-      </c>
-      <c r="H23" t="s">
-        <v>156</v>
-      </c>
-      <c r="J23" t="s">
-        <v>157</v>
       </c>
       <c r="K23" t="s">
         <v>26</v>
@@ -4215,22 +4203,22 @@
         <v>20</v>
       </c>
       <c r="D24" t="s">
+        <v>156</v>
+      </c>
+      <c r="E24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F24" t="s">
         <v>158</v>
       </c>
-      <c r="E24" t="s">
+      <c r="G24" t="s">
         <v>159</v>
       </c>
-      <c r="F24" t="s">
+      <c r="I24" t="s">
         <v>160</v>
       </c>
-      <c r="G24" t="s">
+      <c r="J24" t="s">
         <v>161</v>
-      </c>
-      <c r="I24" t="s">
-        <v>162</v>
-      </c>
-      <c r="J24" t="s">
-        <v>163</v>
       </c>
       <c r="K24" t="s">
         <v>26</v>
@@ -4249,22 +4237,22 @@
         <v>36</v>
       </c>
       <c r="D25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" t="s">
+        <v>164</v>
+      </c>
+      <c r="F25" t="s">
         <v>165</v>
       </c>
-      <c r="E25" t="s">
-        <v>166</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>167</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
+        <v>168</v>
+      </c>
+      <c r="J25" t="s">
         <v>169</v>
-      </c>
-      <c r="H25" t="s">
-        <v>170</v>
-      </c>
-      <c r="J25" t="s">
-        <v>171</v>
       </c>
       <c r="K25" t="s">
         <v>26</v>
@@ -4283,7 +4271,7 @@
         <v>2</v>
       </c>
       <c r="I26" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K26" t="s">
         <v>26</v>
@@ -4302,7 +4290,7 @@
         <v>4</v>
       </c>
       <c r="E27" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K27" t="s">
         <v>26</v>
@@ -4333,7 +4321,7 @@
         <v>105</v>
       </c>
       <c r="J28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="K28" t="s">
         <v>26</v>
@@ -4379,7 +4367,7 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="D30" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K30" t="s">
         <v>26</v>

</xml_diff>